<commit_message>
Ajout d'un rapport presque terminer
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travail.xlsx
+++ b/Doccument_théorique/Journal_de_travail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Schwartz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFD6063-0EA3-4E84-B4B1-A69A3D6674D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0DF1CB-69B7-4333-B66A-A24F787FAEB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -360,6 +360,33 @@
     <t>En groupe de 2, nous avons décrit un logo et l'autre devait le dessiner sans commentaire entre les 2. 
 Nous avons refait l'exercice, mais cette fois-ci en décrivant pendant que l'autre dessinait 
 C'était pour nous introduire Les planifications Cascade et Agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai enregister le pseudo de l'utilisateur dans un fihcier et je le ressort dans le tableau des scores </t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>J'ai fait mes logs</t>
+  </si>
+  <si>
+    <t>J'ai ajouter le possibiliter de tomber sur plusieur grille, il y en a 5 en tout</t>
+  </si>
+  <si>
+    <t>J'ai completé mon rapport</t>
+  </si>
+  <si>
+    <t>Faute d'orthographe</t>
+  </si>
+  <si>
+    <t>J'ai corrigé mes fautres</t>
+  </si>
+  <si>
+    <t>Erreur restant</t>
+  </si>
+  <si>
+    <t>J'ai corriger les dernière petit erreur</t>
   </si>
 </sst>
 </file>
@@ -436,8 +463,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L66" totalsRowShown="0">
-  <autoFilter ref="B4:L66" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L74" totalsRowShown="0">
+  <autoFilter ref="B4:L74" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -720,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L66"/>
+  <dimension ref="B4:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="62" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2716,20 +2743,230 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E64" s="3" t="str">
+    <row r="64" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E64" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" t="s">
+        <v>50</v>
+      </c>
+      <c r="I64" t="s">
+        <v>23</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E65" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.0972222222222188E-2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" t="s">
+        <v>109</v>
+      </c>
+      <c r="I65" t="s">
+        <v>23</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E66" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F66" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" t="s">
+        <v>35</v>
+      </c>
+      <c r="I66" t="s">
+        <v>23</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="E67" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" t="s">
+        <v>48</v>
+      </c>
+      <c r="I67" t="s">
+        <v>23</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E68" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" t="s">
+        <v>113</v>
+      </c>
+      <c r="I68" t="s">
+        <v>23</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E69" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F69" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69" t="s">
+        <v>115</v>
+      </c>
+      <c r="I69" t="s">
+        <v>23</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E70" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" s="3" t="str">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E71" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" s="3" t="str">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E72" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E73" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E74" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>

</xml_diff>